<commit_message>
Update POM and test file
</commit_message>
<xml_diff>
--- a/notes_app_testing/03-Test_case/API_test.xlsx
+++ b/notes_app_testing/03-Test_case/API_test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\Hoc tap\Tester\Personal Project\1. Project 1\notes_app_testing\03-Test_case\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FBFEECB-EB5E-492F-BC1A-7240D44CDC1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA05A27C-77F7-41BD-9DA1-33BEA92CF5BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="24" yWindow="24" windowWidth="23016" windowHeight="12336" xr2:uid="{147A3E30-A16C-4F86-A4FD-635609F1CC62}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1039" uniqueCount="362">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1051" uniqueCount="363">
   <si>
     <t>Test case ID</t>
   </si>
@@ -1374,6 +1374,9 @@
   </si>
   <si>
     <t>Postman</t>
+  </si>
+  <si>
+    <t>Chưa check postman script</t>
   </si>
 </sst>
 </file>
@@ -1404,12 +1407,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -1439,7 +1448,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1489,6 +1498,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1496,7 +1508,16 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1810,10 +1831,10 @@
   <dimension ref="A1:R81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="L28" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomRight" activeCell="L34" sqref="L34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1893,8 +1914,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="118.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="8" t="s">
+    <row r="2" spans="1:18" ht="118.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="17" t="s">
         <v>16</v>
       </c>
       <c r="B2" s="9" t="s">
@@ -1940,10 +1961,12 @@
       <c r="P2" s="8" t="s">
         <v>231</v>
       </c>
-      <c r="Q2" s="8"/>
+      <c r="Q2" s="8" t="s">
+        <v>231</v>
+      </c>
       <c r="R2" s="8"/>
     </row>
-    <row r="3" spans="1:18" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>33</v>
       </c>
@@ -1991,12 +2014,12 @@
         <v>231</v>
       </c>
       <c r="Q3" s="8"/>
-      <c r="R3" s="17" t="s">
+      <c r="R3" s="18" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="72" x14ac:dyDescent="0.3">
-      <c r="A4" s="8" t="s">
+    <row r="4" spans="1:18" ht="72" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="17" t="s">
         <v>34</v>
       </c>
       <c r="B4" s="11" t="s">
@@ -2042,10 +2065,12 @@
       <c r="P4" s="8" t="s">
         <v>231</v>
       </c>
-      <c r="Q4" s="8"/>
-      <c r="R4" s="17"/>
-    </row>
-    <row r="5" spans="1:18" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="Q4" s="8" t="s">
+        <v>231</v>
+      </c>
+      <c r="R4" s="18"/>
+    </row>
+    <row r="5" spans="1:18" ht="100.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>27</v>
       </c>
@@ -2095,9 +2120,9 @@
         <v>231</v>
       </c>
       <c r="Q5" s="8"/>
-      <c r="R5" s="17"/>
-    </row>
-    <row r="6" spans="1:18" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="R5" s="18"/>
+    </row>
+    <row r="6" spans="1:18" ht="100.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
         <v>28</v>
       </c>
@@ -2147,9 +2172,9 @@
         <v>231</v>
       </c>
       <c r="Q6" s="8"/>
-      <c r="R6" s="17"/>
-    </row>
-    <row r="7" spans="1:18" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="R6" s="18"/>
+    </row>
+    <row r="7" spans="1:18" ht="100.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
         <v>30</v>
       </c>
@@ -2199,9 +2224,9 @@
         <v>231</v>
       </c>
       <c r="Q7" s="8"/>
-      <c r="R7" s="17"/>
-    </row>
-    <row r="8" spans="1:18" ht="72" x14ac:dyDescent="0.3">
+      <c r="R7" s="18"/>
+    </row>
+    <row r="8" spans="1:18" ht="72" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
         <v>35</v>
       </c>
@@ -2249,9 +2274,9 @@
         <v>231</v>
       </c>
       <c r="Q8" s="8"/>
-      <c r="R8" s="17"/>
-    </row>
-    <row r="9" spans="1:18" ht="72" x14ac:dyDescent="0.3">
+      <c r="R8" s="18"/>
+    </row>
+    <row r="9" spans="1:18" ht="72" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
         <v>36</v>
       </c>
@@ -2299,9 +2324,9 @@
         <v>231</v>
       </c>
       <c r="Q9" s="8"/>
-      <c r="R9" s="17"/>
-    </row>
-    <row r="10" spans="1:18" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="R9" s="18"/>
+    </row>
+    <row r="10" spans="1:18" ht="100.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
         <v>31</v>
       </c>
@@ -2349,9 +2374,9 @@
         <v>231</v>
       </c>
       <c r="Q10" s="8"/>
-      <c r="R10" s="17"/>
-    </row>
-    <row r="11" spans="1:18" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="R10" s="18"/>
+    </row>
+    <row r="11" spans="1:18" ht="86.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
         <v>38</v>
       </c>
@@ -2399,9 +2424,9 @@
         <v>231</v>
       </c>
       <c r="Q11" s="8"/>
-      <c r="R11" s="17"/>
-    </row>
-    <row r="12" spans="1:18" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="R11" s="18"/>
+    </row>
+    <row r="12" spans="1:18" ht="86.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
         <v>39</v>
       </c>
@@ -2451,10 +2476,10 @@
         <v>231</v>
       </c>
       <c r="Q12" s="8"/>
-      <c r="R12" s="17"/>
-    </row>
-    <row r="13" spans="1:18" ht="144" x14ac:dyDescent="0.3">
-      <c r="A13" s="8" t="s">
+      <c r="R12" s="18"/>
+    </row>
+    <row r="13" spans="1:18" ht="144" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="17" t="s">
         <v>40</v>
       </c>
       <c r="B13" s="9" t="s">
@@ -2500,11 +2525,13 @@
       <c r="P13" s="8" t="s">
         <v>231</v>
       </c>
-      <c r="Q13" s="8"/>
+      <c r="Q13" s="8" t="s">
+        <v>231</v>
+      </c>
       <c r="R13" s="8"/>
     </row>
-    <row r="14" spans="1:18" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="8" t="s">
+    <row r="14" spans="1:18" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="17" t="s">
         <v>44</v>
       </c>
       <c r="B14" s="11" t="s">
@@ -2550,7 +2577,9 @@
       <c r="P14" s="8" t="s">
         <v>231</v>
       </c>
-      <c r="Q14" s="8"/>
+      <c r="Q14" s="8" t="s">
+        <v>231</v>
+      </c>
       <c r="R14" s="8"/>
     </row>
     <row r="15" spans="1:18" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
@@ -2570,7 +2599,7 @@
         <v>46</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>62</v>
+        <v>17</v>
       </c>
       <c r="G15" s="8" t="s">
         <v>18</v>
@@ -2603,7 +2632,7 @@
       <c r="Q15" s="8"/>
       <c r="R15" s="8"/>
     </row>
-    <row r="16" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
         <v>48</v>
       </c>
@@ -2653,7 +2682,7 @@
       <c r="Q16" s="8"/>
       <c r="R16" s="8"/>
     </row>
-    <row r="17" spans="1:18" ht="72" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:18" ht="72" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
         <v>49</v>
       </c>
@@ -2703,7 +2732,7 @@
       <c r="Q17" s="8"/>
       <c r="R17" s="8"/>
     </row>
-    <row r="18" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:18" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
         <v>51</v>
       </c>
@@ -2753,7 +2782,7 @@
       <c r="Q18" s="8"/>
       <c r="R18" s="8"/>
     </row>
-    <row r="19" spans="1:18" ht="72" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:18" ht="72" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="s">
         <v>52</v>
       </c>
@@ -2803,7 +2832,7 @@
       <c r="Q19" s="8"/>
       <c r="R19" s="8"/>
     </row>
-    <row r="20" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:18" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="s">
         <v>53</v>
       </c>
@@ -2853,7 +2882,7 @@
       <c r="Q20" s="8"/>
       <c r="R20" s="8"/>
     </row>
-    <row r="21" spans="1:18" ht="72" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:18" ht="72" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" s="8" t="s">
         <v>54</v>
       </c>
@@ -2903,7 +2932,7 @@
       <c r="Q21" s="8"/>
       <c r="R21" s="8"/>
     </row>
-    <row r="22" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:18" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22" s="8" t="s">
         <v>113</v>
       </c>
@@ -2953,7 +2982,7 @@
       <c r="Q22" s="8"/>
       <c r="R22" s="8"/>
     </row>
-    <row r="23" spans="1:18" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:18" ht="86.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" s="8" t="s">
         <v>114</v>
       </c>
@@ -3003,8 +3032,8 @@
       <c r="Q23" s="8"/>
       <c r="R23" s="12"/>
     </row>
-    <row r="24" spans="1:18" ht="100.8" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="8" t="s">
+    <row r="24" spans="1:18" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A24" s="17" t="s">
         <v>115</v>
       </c>
       <c r="B24" s="11" t="s">
@@ -3050,8 +3079,12 @@
       <c r="P24" s="8" t="s">
         <v>231</v>
       </c>
-      <c r="Q24" s="8"/>
-      <c r="R24" s="12"/>
+      <c r="Q24" s="8" t="s">
+        <v>231</v>
+      </c>
+      <c r="R24" s="12" t="s">
+        <v>362</v>
+      </c>
     </row>
     <row r="25" spans="1:18" ht="86.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" s="8" t="s">
@@ -3207,8 +3240,8 @@
       <c r="Q27" s="8"/>
       <c r="R27" s="12"/>
     </row>
-    <row r="28" spans="1:18" ht="86.4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="8" t="s">
+    <row r="28" spans="1:18" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A28" s="17" t="s">
         <v>117</v>
       </c>
       <c r="B28" s="11" t="s">
@@ -3254,8 +3287,12 @@
       <c r="P28" s="8" t="s">
         <v>231</v>
       </c>
-      <c r="Q28" s="8"/>
-      <c r="R28" s="12"/>
+      <c r="Q28" s="8" t="s">
+        <v>231</v>
+      </c>
+      <c r="R28" s="12" t="s">
+        <v>362</v>
+      </c>
     </row>
     <row r="29" spans="1:18" ht="144" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" s="8" t="s">
@@ -3517,8 +3554,8 @@
       <c r="Q33" s="8"/>
       <c r="R33" s="12"/>
     </row>
-    <row r="34" spans="1:18" ht="115.2" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="8" t="s">
+    <row r="34" spans="1:18" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A34" s="17" t="s">
         <v>84</v>
       </c>
       <c r="B34" s="11" t="s">
@@ -3567,8 +3604,8 @@
       <c r="Q34" s="8"/>
       <c r="R34" s="12"/>
     </row>
-    <row r="35" spans="1:18" ht="129.6" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="8" t="s">
+    <row r="35" spans="1:18" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A35" s="17" t="s">
         <v>121</v>
       </c>
       <c r="B35" s="11" t="s">
@@ -3616,7 +3653,9 @@
       <c r="P35" s="8" t="s">
         <v>231</v>
       </c>
-      <c r="Q35" s="8"/>
+      <c r="Q35" s="8" t="s">
+        <v>231</v>
+      </c>
       <c r="R35" s="12"/>
     </row>
     <row r="36" spans="1:18" ht="86.4" hidden="1" x14ac:dyDescent="0.3">
@@ -3723,8 +3762,8 @@
       <c r="Q37" s="8"/>
       <c r="R37" s="8"/>
     </row>
-    <row r="38" spans="1:18" ht="162" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="8" t="s">
+    <row r="38" spans="1:18" ht="162" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="17" t="s">
         <v>124</v>
       </c>
       <c r="B38" s="11" t="s">
@@ -3770,7 +3809,9 @@
       <c r="P38" s="8" t="s">
         <v>231</v>
       </c>
-      <c r="Q38" s="8"/>
+      <c r="Q38" s="8" t="s">
+        <v>231</v>
+      </c>
       <c r="R38" s="13" t="s">
         <v>224</v>
       </c>
@@ -4037,8 +4078,8 @@
       <c r="Q43" s="8"/>
       <c r="R43" s="8"/>
     </row>
-    <row r="44" spans="1:18" ht="86.4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="8" t="s">
+    <row r="44" spans="1:18" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A44" s="17" t="s">
         <v>128</v>
       </c>
       <c r="B44" s="11" t="s">
@@ -4084,7 +4125,9 @@
       <c r="P44" s="8" t="s">
         <v>231</v>
       </c>
-      <c r="Q44" s="8"/>
+      <c r="Q44" s="8" t="s">
+        <v>231</v>
+      </c>
       <c r="R44" s="12"/>
     </row>
     <row r="45" spans="1:18" ht="144" hidden="1" x14ac:dyDescent="0.3">
@@ -4499,8 +4542,8 @@
       <c r="Q52" s="8"/>
       <c r="R52" s="8"/>
     </row>
-    <row r="53" spans="1:18" ht="86.4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="8" t="s">
+    <row r="53" spans="1:18" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A53" s="17" t="s">
         <v>136</v>
       </c>
       <c r="B53" s="11" t="s">
@@ -4876,7 +4919,7 @@
         <v>106</v>
       </c>
       <c r="F60" s="8" t="s">
-        <v>62</v>
+        <v>17</v>
       </c>
       <c r="G60" s="8" t="s">
         <v>18</v>
@@ -4910,7 +4953,7 @@
       <c r="R60" s="8"/>
     </row>
     <row r="61" spans="1:18" ht="72" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="8" t="s">
+      <c r="A61" s="17" t="s">
         <v>144</v>
       </c>
       <c r="B61" s="11" t="s">
@@ -4926,7 +4969,7 @@
         <v>106</v>
       </c>
       <c r="F61" s="8" t="s">
-        <v>62</v>
+        <v>17</v>
       </c>
       <c r="G61" s="8" t="s">
         <v>18</v>
@@ -4956,7 +4999,9 @@
       <c r="P61" s="8" t="s">
         <v>231</v>
       </c>
-      <c r="Q61" s="8"/>
+      <c r="Q61" s="8" t="s">
+        <v>231</v>
+      </c>
       <c r="R61" s="8"/>
     </row>
     <row r="62" spans="1:18" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
@@ -4976,7 +5021,7 @@
         <v>106</v>
       </c>
       <c r="F62" s="8" t="s">
-        <v>62</v>
+        <v>17</v>
       </c>
       <c r="G62" s="8" t="s">
         <v>18</v>
@@ -5026,7 +5071,7 @@
         <v>106</v>
       </c>
       <c r="F63" s="8" t="s">
-        <v>62</v>
+        <v>17</v>
       </c>
       <c r="G63" s="8" t="s">
         <v>18</v>
@@ -5078,7 +5123,7 @@
         <v>110</v>
       </c>
       <c r="F64" s="8" t="s">
-        <v>62</v>
+        <v>17</v>
       </c>
       <c r="G64" s="8" t="s">
         <v>18</v>
@@ -5128,7 +5173,7 @@
         <v>110</v>
       </c>
       <c r="F65" s="8" t="s">
-        <v>62</v>
+        <v>17</v>
       </c>
       <c r="G65" s="8" t="s">
         <v>18</v>
@@ -5436,10 +5481,11 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:R67" xr:uid="{C0183FFE-7F6B-4E86-854D-1FBC1023561F}">
-    <filterColumn colId="5">
-      <filters>
-        <filter val="Authentication"/>
-      </filters>
+    <filterColumn colId="0">
+      <colorFilter dxfId="0"/>
+    </filterColumn>
+    <filterColumn colId="16">
+      <filters blank="1"/>
     </filterColumn>
   </autoFilter>
   <mergeCells count="1">
@@ -5454,5 +5500,6 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>